<commit_message>
Apex Sharing best practices
</commit_message>
<xml_diff>
--- a/Notes/URLs.xlsx
+++ b/Notes/URLs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nsiripurapu\Desktop\Apex Enterprise Patterns\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F923E2D-8920-43E6-AFBE-B651EDD6BE4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CE525E-F271-49B6-ADF0-A879124BC43E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="102">
   <si>
     <t>https://blog.texei.com/refresh-a-record-page-from-a-lightning-web-component-14a5874ff68e</t>
   </si>
@@ -340,6 +340,12 @@
   </si>
   <si>
     <t>debug-log-analyzer</t>
+  </si>
+  <si>
+    <t>rfLib</t>
+  </si>
+  <si>
+    <t>Logging Framework for Apex, AURA and LWC components</t>
   </si>
 </sst>
 </file>
@@ -1159,10 +1165,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A900DDA-61E7-42E2-A62B-3EE2124DC406}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1179,6 +1185,14 @@
         <v>89</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1188,7 +1202,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E21982E-477D-433F-A1B0-FB62CD8142DB}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>